<commit_message>
Se agregaron las paginas de navegacion y lecturas de db
</commit_message>
<xml_diff>
--- a/Modelo de dominio.xlsx
+++ b/Modelo de dominio.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1711CC73-B04B-4500-A30E-0016E1EA09A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Marca</t>
   </si>
@@ -27,9 +33,6 @@
     <t>Categoria</t>
   </si>
   <si>
-    <t>El usuario podrá en todo momento dar de alta nuevas marcas, tipos, productos, proveedores y realizar nuevas asociaciones o modificar las existente</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -72,18 +75,12 @@
     <t>VENTAS (FORMULARIO)</t>
   </si>
   <si>
-    <t>El sistema debe manejar seguridad (ingreso con usuario y  contraseña), con un perfil vendedor que registra ventas y un perfil administrador que puede hacer todo.</t>
-  </si>
-  <si>
     <t>PRECIO PARCIAL</t>
   </si>
   <si>
     <t>PRECIO FINAL</t>
   </si>
   <si>
-    <t>PREGUNTAS</t>
-  </si>
-  <si>
     <t>IDPROVEEDOR</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
   </si>
   <si>
     <t>ID(NUM UNICO)</t>
-  </si>
-  <si>
-    <t>PRECIO VENTA</t>
   </si>
   <si>
     <t>FECHA COMPRA</t>
@@ -144,8 +138,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,13 +181,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -262,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,9 +323,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -328,10 +333,16 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -354,15 +365,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>1463039</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>178904</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -370,7 +381,7 @@
         <xdr:cNvPr id="4" name="Rectángulo 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -421,13 +432,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>769620</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -437,7 +448,7 @@
         <xdr:cNvPr id="5" name="Rectángulo 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -492,13 +503,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>1905</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
@@ -508,7 +519,7 @@
         <xdr:cNvPr id="6" name="Rectángulo 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -518,77 +529,6 @@
         <a:xfrm>
           <a:off x="3009900" y="2409825"/>
           <a:ext cx="1150620" cy="1483995"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="95000"/>
-              <a:lumOff val="5000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-ES" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="es-ES" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>185530</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rectángulo 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="2246243"/>
-          <a:ext cx="781878" cy="572743"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -636,21 +576,21 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>6235</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Rectángulo 7">
+        <xdr:cNvPr id="7" name="Rectángulo 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -658,8 +598,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="762000" y="2705100"/>
-          <a:ext cx="762000" cy="561975"/>
+          <a:off x="0" y="2184659"/>
+          <a:ext cx="788894" cy="550137"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -705,259 +645,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>93718</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="Conector recto de flecha 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000A000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="7" idx="3"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="784860" y="2501638"/>
-          <a:ext cx="2225040" cy="508262"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>14</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>104772</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>632461</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="12" name="Conector recto de flecha 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00000C000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="1569734" y="3244212"/>
-          <a:ext cx="1417307" cy="24768"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>2</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>85642</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="17" name="Conector recto de flecha 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000011000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="4" idx="3"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="7292340" y="3048000"/>
-          <a:ext cx="784862" cy="542842"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>13335</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>104776</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>737235</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="Conector recto de flecha 29">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00001E000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2367915" y="851536"/>
-          <a:ext cx="723900" cy="66674"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>19879</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="36" name="Rectángulo 35">
+        <xdr:cNvPr id="8" name="Rectángulo 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000024000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -965,8 +669,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4916558" y="377689"/>
-          <a:ext cx="1464365" cy="967407"/>
+          <a:off x="762000" y="2705100"/>
+          <a:ext cx="762000" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1012,36 +716,96 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>93718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="37" name="Conector recto de flecha 36">
+        <xdr:cNvPr id="10" name="Conector recto de flecha 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000025000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="7" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="788894" y="2460400"/>
+          <a:ext cx="2232212" cy="497505"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>14</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104772</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>632461</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Conector recto de flecha 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2369820" y="832485"/>
-          <a:ext cx="2438400" cy="180975"/>
+        <a:xfrm rot="10800000">
+          <a:off x="1569734" y="3244212"/>
+          <a:ext cx="1417307" cy="24768"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 4063"/>
+            <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1072,21 +836,139 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>6627</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>17930</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>17929</xdr:rowOff>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>85642</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Conector recto de flecha 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="4" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="7292340" y="3048000"/>
+          <a:ext cx="784862" cy="542842"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>13335</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>737235</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Conector recto de flecha 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2367915" y="851536"/>
+          <a:ext cx="723900" cy="66674"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19879</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="Rectángulo 28">
+        <xdr:cNvPr id="36" name="Rectángulo 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5743CFE0-37AF-471D-8A81-A43C96AD1AB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000024000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1094,8 +976,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8095129" y="2552603"/>
-          <a:ext cx="1846730" cy="907773"/>
+          <a:off x="4916558" y="377689"/>
+          <a:ext cx="1464365" cy="967407"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1141,93 +1023,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>701040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="43" name="CuadroTexto 42">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3D66BF6F-CB97-4550-8733-5A1420BBF1A6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3055620" y="556260"/>
-          <a:ext cx="1242060" cy="243840"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES" sz="800"/>
-            <a:t>DEBE ESTAR REGISTRADO</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>19879</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>106017</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>6626</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>79514</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="33" name="Conector recto de flecha 23">
+        <xdr:cNvPr id="37" name="Conector recto de flecha 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000025000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1235,12 +1047,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4154557" y="1239078"/>
-          <a:ext cx="5744817" cy="1278836"/>
+          <a:off x="2369820" y="832485"/>
+          <a:ext cx="2438400" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 110092"/>
+            <a:gd name="adj1" fmla="val 4063"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1269,23 +1081,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>779930</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>179294</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>6627</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1819836</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>28843</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>17930</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>17929</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="60" name="Rectángulo 35">
+        <xdr:cNvPr id="29" name="Rectángulo 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000024000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1293,8 +1105,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8086165" y="905435"/>
-          <a:ext cx="1828800" cy="943243"/>
+          <a:off x="8095129" y="2552603"/>
+          <a:ext cx="1846730" cy="907773"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1340,95 +1152,110 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1457739</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>99393</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>6626</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>79514</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="CuadroTexto 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3055620" y="556260"/>
+          <a:ext cx="1242060" cy="243840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="800"/>
+            <a:t>DEBE ESTAR REGISTRADO</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28844</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>98612</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>178126</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="61" name="Conector recto de flecha 23">
+        <xdr:cNvPr id="33" name="Conector recto de flecha 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="6374296" y="655984"/>
-          <a:ext cx="1696278" cy="742121"/>
+        <a:xfrm flipV="1">
+          <a:off x="4188468" y="1013012"/>
+          <a:ext cx="7053273" cy="1531796"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj1" fmla="val 105543"/>
           </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>583097</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>82661</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>712304</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>178905</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="97" name="Conector recto de flecha 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000016000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:endCxn id="98" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10507026" y="2449343"/>
-          <a:ext cx="918102" cy="96244"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
         </a:prstGeom>
         <a:ln>
           <a:solidFill>
@@ -1457,22 +1284,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>19877</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>178905</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1404731</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>37808</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="98" name="Rectángulo 28">
+        <xdr:cNvPr id="60" name="Rectángulo 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5743CFE0-37AF-471D-8A81-A43C96AD1AB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1480,8 +1307,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10732701" y="2545587"/>
-          <a:ext cx="1384854" cy="896860"/>
+          <a:off x="8292353" y="914400"/>
+          <a:ext cx="1828800" cy="943243"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1527,23 +1354,141 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>17930</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>116542</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1084729</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>13252</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104070</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="Conector recto de flecha 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00003D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="60" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="6427695" y="475130"/>
+          <a:ext cx="3693459" cy="910893"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 8981"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>609991</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1978</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>712304</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>178905</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="97" name="Conector recto de flecha 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000061000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="98" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10731144" y="2547954"/>
+          <a:ext cx="891207" cy="176927"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19877</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>178905</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1404731</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="99" name="Rectángulo 7">
+        <xdr:cNvPr id="98" name="Rectángulo 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000062000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1551,8 +1496,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6409765" y="1461247"/>
-          <a:ext cx="1084729" cy="371840"/>
+          <a:off x="10732701" y="2545587"/>
+          <a:ext cx="1384854" cy="896860"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1601,71 +1546,20 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>132521</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>13252</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>132522</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="105" name="Straight Connector 104"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7282070" y="1636643"/>
-          <a:ext cx="795130" cy="1"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>19878</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>13253</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>13252</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>33132</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1084729</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>13252</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="116" name="Rectángulo 7">
+        <xdr:cNvPr id="99" name="Rectángulo 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000063000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1673,8 +1567,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6400800" y="2073966"/>
-          <a:ext cx="1676400" cy="397566"/>
+          <a:off x="6409765" y="1461247"/>
+          <a:ext cx="1084729" cy="371840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1721,81 +1615,38 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1084729</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>132521</xdr:rowOff>
+      <xdr:rowOff>125506</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>13252</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>132522</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1810871</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>6626</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="117" name="Straight Connector 104"/>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvPr id="117" name="Straight Connector 104">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000075000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="99" idx="3"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7282070" y="1636643"/>
-          <a:ext cx="795130" cy="1"/>
+        <a:xfrm flipV="1">
+          <a:off x="7494494" y="1586753"/>
+          <a:ext cx="2608730" cy="60414"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
             <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
-        </a:prstGeom>
-        <a:ln w="12700">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>957859</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>119277</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>19878</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>13254</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="118" name="Straight Connector 104"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="116" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="7713645" y="1413797"/>
-          <a:ext cx="252565" cy="944607"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
         </a:prstGeom>
         <a:ln w="12700">
           <a:solidFill>
@@ -1823,31 +1674,90 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>24384</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>99392</xdr:rowOff>
+      <xdr:colOff>877177</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>119277</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1821784</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>13254</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="118" name="Straight Connector 104">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000076000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="9515551" y="1413797"/>
+          <a:ext cx="252565" cy="944607"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>100583</xdr:rowOff>
+      <xdr:colOff>17929</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>80682</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19877</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>89452</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="124" name="Conector recto de flecha 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00007C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="98" idx="1"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="9939528" y="2879168"/>
-          <a:ext cx="768096" cy="1191"/>
+        <a:xfrm rot="10800000">
+          <a:off x="10139082" y="2985247"/>
+          <a:ext cx="1122536" cy="188064"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1876,6 +1786,77 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19878</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>13253</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>8965</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>26894</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rectángulo 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B23BA59-827A-4516-8A83-CE06832969DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8312231" y="2012382"/>
+          <a:ext cx="1817887" cy="381194"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2136,279 +2117,270 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="11"/>
-    <col min="2" max="3" width="11.44140625" style="2"/>
-    <col min="4" max="4" width="9.5546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" style="2"/>
-    <col min="7" max="7" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="2"/>
-    <col min="10" max="10" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="11"/>
+    <col min="3" max="4" width="11.44140625" style="2"/>
+    <col min="5" max="5" width="9.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" style="2"/>
+    <col min="8" max="8" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="2"/>
+    <col min="11" max="11" width="26.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="18"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="H3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3"/>
+    </row>
+    <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4"/>
+    </row>
+    <row r="5" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5"/>
+    </row>
+    <row r="6" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="20"/>
+      <c r="D6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="3"/>
+      <c r="I9" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="H10" s="3"/>
+      <c r="I10" s="22"/>
+      <c r="L10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I11" s="13"/>
+    </row>
+    <row r="12" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="14"/>
+    </row>
+    <row r="13" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="14"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="K16" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C17" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="K17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C18" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="K18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="K19" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="F20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="19"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="G3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3"/>
-    </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1">
-      <c r="G4" s="6" t="s">
+      <c r="K20" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="J4"/>
-    </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1">
-      <c r="A5" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5"/>
-    </row>
-    <row r="6" spans="1:12" ht="15" thickBot="1">
-      <c r="A6" s="21"/>
-      <c r="C6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="C7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="12" t="s">
+      <c r="I21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K21" s="3"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D22" s="14"/>
+      <c r="F22" s="16"/>
+      <c r="I22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="3"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D23" s="14"/>
+      <c r="F23" s="16"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D24" s="14"/>
+    </row>
+    <row r="25" spans="2:13" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="2:13" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="2:13" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="B27" s="4"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B29" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="C8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="14.4" customHeight="1">
-      <c r="G9" s="3"/>
-      <c r="H9" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="G10" s="3"/>
-      <c r="H10" s="22"/>
-      <c r="J10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="1:12" ht="14.4" customHeight="1">
-      <c r="H12" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="23"/>
-    </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1">
-      <c r="A13" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="14"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="J15" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="L15" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="E16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="J16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="B17" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="J17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="B18" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="J18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="B19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J19" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="E20" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J20" s="3"/>
-      <c r="L20" s="2"/>
-    </row>
-    <row r="21" spans="1:12" ht="14.4" customHeight="1">
-      <c r="E21" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J21" s="3"/>
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="C22" s="14"/>
-      <c r="E22" s="16"/>
-      <c r="J22" s="18"/>
-      <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="C23" s="14"/>
-      <c r="E23" s="16"/>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="C24" s="14"/>
-    </row>
-    <row r="25" spans="1:12" ht="16.8">
-      <c r="A25" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="16.8">
-      <c r="A26" s="4"/>
-    </row>
-    <row r="27" spans="1:12" ht="16.8">
-      <c r="A27" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="11" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="H12:I13"/>
+  <mergeCells count="5">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I12:J13"/>
+    <mergeCell ref="K12:K13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>